<commit_message>
data: add 2023-03-27 notices
</commit_message>
<xml_diff>
--- a/data/position_notices/2023-03-27.xlsx
+++ b/data/position_notices/2023-03-27.xlsx
@@ -464,41 +464,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>股票名称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>股票代码</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>公告标题</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>公告日期</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>公告发布时间</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>公告链接</t>
         </is>
@@ -507,17 +507,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>*ST中安</t>
+          <t>山东路桥</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>600654</t>
+          <t>000498</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>*ST中安:监事会关于对2023年股票期权与限制性股票激励计划首次授予激励对象名单审核意见及公示情况的说明</t>
+          <t>山东路桥:向不特定对象发行可转换公司债券网上中签号码公告</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -527,12 +527,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-03-27 16:51:25:000</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577186.html</t>
+          <t>2023-03-27 15:45:38:000</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/000498/AN202303271584574814.html</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>*ST中安:*ST中安2023年第一次临时股东大会会议资料</t>
+          <t>*ST中安:监事会关于对2023年股票期权与限制性股票激励计划首次授予激励对象名单审核意见及公示情况的说明</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -562,9 +562,9 @@
           <t>2023-03-27 16:51:25:000</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577189.html</t>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577186.html</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>*ST中安:关于公司股票可能被终止上市的第五次风险提示公告</t>
+          <t>*ST中安:*ST中安2023年第一次临时股东大会会议资料</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -594,9 +594,9 @@
           <t>2023-03-27 16:51:25:000</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577190.html</t>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577189.html</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>*ST中安:第十一届监事会第六次会议决议公告</t>
+          <t>*ST中安:关于公司股票可能被终止上市的第五次风险提示公告</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -626,26 +626,26 @@
           <t>2023-03-27 16:51:25:000</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577187.html</t>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577190.html</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>桐昆股份</t>
+          <t>*ST中安</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>601233</t>
+          <t>600654</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>桐昆股份:桐昆集团股份有限公司独立董事独立意见</t>
+          <t>*ST中安:第十一届监事会第六次会议决议公告</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -655,12 +655,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-03-27 16:11:27:000</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575460.html</t>
+          <t>2023-03-27 16:51:25:000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600654/AN202303271584577187.html</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>桐昆股份:关于收购广西桐昆石化有限公司部分股权暨关联交易的公告</t>
+          <t>桐昆股份:桐昆集团股份有限公司独立董事独立意见</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -690,9 +690,9 @@
           <t>2023-03-27 16:11:27:000</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575455.html</t>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575460.html</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>桐昆股份:国信证券关于桐昆股份收购广西桐昆石化有限公司股权暨关联交易的核查意见</t>
+          <t>桐昆股份:关于收购广西桐昆石化有限公司部分股权暨关联交易的公告</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -722,9 +722,9 @@
           <t>2023-03-27 16:11:27:000</t>
         </is>
       </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575457.html</t>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575455.html</t>
         </is>
       </c>
     </row>
@@ -741,7 +741,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>桐昆股份:桐昆股份第八届监事会第十八次会议决议公告</t>
+          <t>桐昆股份:国信证券关于桐昆股份收购广西桐昆石化有限公司股权暨关联交易的核查意见</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -754,9 +754,9 @@
           <t>2023-03-27 16:11:27:000</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575458.html</t>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575457.html</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>桐昆股份:桐昆股份第八届董事会第二十五次会议决议公告</t>
+          <t>桐昆股份:桐昆股份第八届监事会第十八次会议决议公告</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -786,26 +786,26 @@
           <t>2023-03-27 16:11:27:000</t>
         </is>
       </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575459.html</t>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575458.html</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>海螺水泥</t>
+          <t>桐昆股份</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>600585</t>
+          <t>601233</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>海螺水泥:董事会审核委员会2022年度履职报告</t>
+          <t>桐昆股份:桐昆股份第八届董事会第二十五次会议决议公告</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -815,12 +815,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:21:000</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586401.html</t>
+          <t>2023-03-27 16:11:27:000</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/601233/AN202303271584575459.html</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年度非经营性资金占用及其他关联资金往来情况的专项说明</t>
+          <t>海螺水泥:董事会审核委员会2022年度履职报告</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -847,12 +847,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:58:000</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586408.html</t>
+          <t>2023-03-27 19:52:21:000</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586401.html</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年度独立非执行董事述职报告</t>
+          <t>海螺水泥:2022年度非经营性资金占用及其他关联资金往来情况的专项说明</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -879,12 +879,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2023-03-27 19:51:48:000</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586397.html</t>
+          <t>2023-03-27 19:52:58:000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586408.html</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>海螺水泥:关于续聘会计师事务所的公告</t>
+          <t>海螺水泥:2022年度独立非执行董事述职报告</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -911,12 +911,12 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:21:000</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586410.html</t>
+          <t>2023-03-27 19:51:48:000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586397.html</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>海螺水泥:董事会决议公告</t>
+          <t>海螺水泥:关于续聘会计师事务所的公告</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -943,12 +943,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2023-03-27 19:51:32:000</t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586396.html</t>
+          <t>2023-03-27 19:52:21:000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586410.html</t>
         </is>
       </c>
     </row>
@@ -965,7 +965,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年度中国准则审计报告(含财务报告)</t>
+          <t>海螺水泥:董事会决议公告</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -975,12 +975,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:58:000</t>
-        </is>
-      </c>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586406.html</t>
+          <t>2023-03-27 19:51:32:000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586396.html</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>海螺水泥:安徽海螺水泥股份有限公司独立董事工作制度</t>
+          <t>海螺水泥:2022年度中国准则审计报告(含财务报告)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1007,12 +1007,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:21:000</t>
-        </is>
-      </c>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586413.html</t>
+          <t>2023-03-27 19:52:58:000</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586406.html</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>海螺水泥:关于为附属公司及合营公司提供担保额度预计的公告</t>
+          <t>海螺水泥:安徽海螺水泥股份有限公司独立董事工作制度</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1042,9 +1042,9 @@
           <t>2023-03-27 19:52:21:000</t>
         </is>
       </c>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586402.html</t>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586413.html</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年年度报告</t>
+          <t>海螺水泥:关于为附属公司及合营公司提供担保额度预计的公告</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1071,12 +1071,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2023-03-27 19:51:32:000</t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586394.html</t>
+          <t>2023-03-27 19:52:21:000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586402.html</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>海螺水泥:监事会决议公告</t>
+          <t>海螺水泥:2022年年度报告</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1103,12 +1103,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:21:000</t>
-        </is>
-      </c>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586399.html</t>
+          <t>2023-03-27 19:51:32:000</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586394.html</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年内部控制评价报告</t>
+          <t>海螺水泥:监事会决议公告</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1138,9 +1138,9 @@
           <t>2023-03-27 19:52:21:000</t>
         </is>
       </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586404.html</t>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586399.html</t>
         </is>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>海螺水泥:关于修订《公司章程》部分条款的公告</t>
+          <t>海螺水泥:2022年内部控制评价报告</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1170,9 +1170,9 @@
           <t>2023-03-27 19:52:21:000</t>
         </is>
       </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586409.html</t>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586404.html</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年度环境、社会及管治报告</t>
+          <t>海螺水泥:关于修订《公司章程》部分条款的公告</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1199,12 +1199,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2023-03-27 19:54:40:000</t>
-        </is>
-      </c>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586412.html</t>
+          <t>2023-03-27 19:52:21:000</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586409.html</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>海螺水泥:独立董事对公司对外担保情况的专项说明</t>
+          <t>海螺水泥:2022年度环境、社会及管治报告</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1231,12 +1231,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2023-03-27 19:52:21:000</t>
-        </is>
-      </c>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586398.html</t>
+          <t>2023-03-27 19:54:40:000</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586412.html</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年年度报告摘要</t>
+          <t>海螺水泥:独立董事对公司对外担保情况的专项说明</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1263,12 +1263,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2023-03-27 19:51:32:000</t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586395.html</t>
+          <t>2023-03-27 19:52:21:000</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586398.html</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1285,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>海螺水泥:2022年度内部控制审计报告</t>
+          <t>海螺水泥:2022年年度报告摘要</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1295,12 +1295,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2023-03-27 19:53:22:000</t>
-        </is>
-      </c>
-      <c r="F26" s="2" t="inlineStr">
-        <is>
-          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586403.html</t>
+          <t>2023-03-27 19:51:32:000</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586395.html</t>
         </is>
       </c>
     </row>
@@ -1317,55 +1317,59 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>海螺水泥:2022年度内部控制审计报告</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2023-03-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2023-03-27 19:53:22:000</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586403.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>海螺水泥</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>600585</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>海螺水泥:2022年年度利润分配方案公告</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>2023-03-28 00:00:00</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2023-03-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>2023-03-27 19:52:21:000</t>
         </is>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>https://data.eastmoney.com/notices/detail/600585/AN202303271584586400.html</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F21" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F22" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F23" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F24" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F25" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F26" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="F27" r:id="rId26"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1375,7 +1379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1403,45 +1407,60 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>*ST中安</t>
+          <t>山东路桥</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>600654</t>
+          <t>000498</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>桐昆股份</t>
+          <t>*ST中安</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>601233</t>
+          <t>600654</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>海螺水泥</t>
+          <t>桐昆股份</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>600585</t>
+          <t>601233</t>
         </is>
       </c>
       <c r="C4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>海螺水泥</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>600585</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>17</v>
       </c>
     </row>

</xml_diff>